<commit_message>
just deleted some shit
</commit_message>
<xml_diff>
--- a/LIFESPAN url CHECK.xlsx
+++ b/LIFESPAN url CHECK.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="195">
   <si>
     <t>Destination URL</t>
   </si>
@@ -31,27 +31,6 @@
   </si>
   <si>
     <t>http://www.lifespanfitness.com/wps/configure-desk/tr1200-dt5-treadmill-desk-2tandems.html?_oskwdid=13325685&amp;_engineadid={creative}</t>
-  </si>
-  <si>
-    <t>http://www.lifespanfitness.com/wps/configure-desk/tr1200-dt5-treadmill-desk-2tandems.html?_oskwdid=13325719&amp;_engineadid={creative}</t>
-  </si>
-  <si>
-    <t>http://www.lifespanfitness.com/wps/configure-desk/tr1200-dt5-treadmill-desk-2tandems.html?_oskwdid=13325753&amp;_engineadid={creative}</t>
-  </si>
-  <si>
-    <t>http://www.lifespanfitness.com/wps/configure-desk/tr1200-dt5-treadmill-desk-2tandems.html?_oskwdid=13325769&amp;_engineadid={creative}</t>
-  </si>
-  <si>
-    <t>http://www.lifespanfitness.com/wps/configure-desk/tr800-dt5-treadmill-desk-1tandem.html?_oskwdid=13325819&amp;_engineadid={creative}</t>
-  </si>
-  <si>
-    <t>http://www.lifespanfitness.com/wps/configure-desk/tr800-dt5-treadmill-desk-1tandem.html?_oskwdid=13325822&amp;_engineadid={creative}</t>
-  </si>
-  <si>
-    <t>http://www.lifespanfitness.com/wps/configure-desk/tr800-dt5-treadmill-desk-1tandem.html?_oskwdid=13325823&amp;_engineadid={creative}</t>
-  </si>
-  <si>
-    <t>http://www.lifespanfitness.com/wps/configure-desk/tr800-dt5-treadmill-desk-1tandem.html?_oskwdid=13325827&amp;_engineadid={creative}</t>
   </si>
   <si>
     <t>http://www.lifespanfitness.com/wps/configure-desk/tr800-dt5-treadmill-desk-1tandem.html?_oskwdid=13325830&amp;_engineadid={creative}</t>
@@ -960,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A221"/>
+  <dimension ref="A1:A214"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1838,38 +1817,38 @@
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
         <v>180</v>
       </c>
     </row>
@@ -1928,54 +1907,19 @@
         <v>191</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
-        <v>197</v>
-      </c>
-    </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
-        <v>201</v>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>